<commit_message>
updated coordsToU to have start/end point visualization also made it able to toggle figure generation entirely made multiObstacleReset's function call comply to this
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -13,7 +13,91 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="588">
+  <si>
+    <t>methodN</t>
+  </si>
+  <si>
+    <t>pathDist</t>
+  </si>
+  <si>
+    <t>numIterations</t>
+  </si>
+  <si>
+    <t>calcTime</t>
+  </si>
+  <si>
+    <t>kGoal</t>
+  </si>
+  <si>
+    <t>kObst</t>
+  </si>
+  <si>
+    <t>rObst</t>
+  </si>
+  <si>
+    <t>methodN</t>
+  </si>
+  <si>
+    <t>pathDist</t>
+  </si>
+  <si>
+    <t>numIterations</t>
+  </si>
+  <si>
+    <t>calcTime</t>
+  </si>
+  <si>
+    <t>kGoal</t>
+  </si>
+  <si>
+    <t>kObst</t>
+  </si>
+  <si>
+    <t>rObst</t>
+  </si>
+  <si>
+    <t>methodN</t>
+  </si>
+  <si>
+    <t>pathDist</t>
+  </si>
+  <si>
+    <t>numIterations</t>
+  </si>
+  <si>
+    <t>calcTime</t>
+  </si>
+  <si>
+    <t>kGoal</t>
+  </si>
+  <si>
+    <t>kObst</t>
+  </si>
+  <si>
+    <t>rObst</t>
+  </si>
+  <si>
+    <t>methodN</t>
+  </si>
+  <si>
+    <t>pathDist</t>
+  </si>
+  <si>
+    <t>numIterations</t>
+  </si>
+  <si>
+    <t>calcTime</t>
+  </si>
+  <si>
+    <t>kGoal</t>
+  </si>
+  <si>
+    <t>kObst</t>
+  </si>
+  <si>
+    <t>rObst</t>
+  </si>
   <si>
     <t>methodN</t>
   </si>
@@ -1713,7 +1797,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="81">
+  <borders count="85">
     <border>
       <left/>
       <right/>
@@ -1801,11 +1885,15 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1887,6 +1975,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="78" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="79" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="80" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="81" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="82" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="83" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="84" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1910,25 +2002,25 @@
   <sheetData>
     <row r="2">
       <c r="B2" s="0" t="s">
-        <v>532</v>
+        <v>560</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>533</v>
+        <v>561</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>534</v>
+        <v>562</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>535</v>
+        <v>563</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>536</v>
+        <v>564</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>537</v>
+        <v>565</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>538</v>
+        <v>566</v>
       </c>
     </row>
     <row r="3">
@@ -1942,7 +2034,7 @@
         <v>281</v>
       </c>
       <c r="E3" s="0">
-        <v>0.0108287</v>
+        <v>0.1643925</v>
       </c>
       <c r="F3" s="0">
         <v>0.0025000000000000001</v>
@@ -1965,7 +2057,7 @@
         <v>306</v>
       </c>
       <c r="E4" s="0">
-        <v>0.0138475</v>
+        <v>0.015528999999999999</v>
       </c>
       <c r="F4" s="0">
         <v>0.0025000000000000001</v>
@@ -1988,7 +2080,7 @@
         <v>355</v>
       </c>
       <c r="E5" s="0">
-        <v>0.031526199999999997</v>
+        <v>0.023719299999999999</v>
       </c>
       <c r="F5" s="0">
         <v>0.01</v>
@@ -2002,25 +2094,25 @@
     </row>
     <row r="10">
       <c r="B10" s="0" t="s">
-        <v>539</v>
+        <v>567</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>540</v>
+        <v>568</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>541</v>
+        <v>569</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>542</v>
+        <v>570</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>543</v>
+        <v>571</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>544</v>
+        <v>572</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>545</v>
+        <v>573</v>
       </c>
     </row>
     <row r="11">
@@ -2034,7 +2126,7 @@
         <v>291</v>
       </c>
       <c r="E11" s="0">
-        <v>0.0091156999999999992</v>
+        <v>0.012711099999999999</v>
       </c>
       <c r="F11" s="0">
         <v>0.0025000000000000001</v>
@@ -2057,7 +2149,7 @@
         <v>313</v>
       </c>
       <c r="E12" s="0">
-        <v>0.013849800000000001</v>
+        <v>0.0225343</v>
       </c>
       <c r="F12" s="0">
         <v>0.0025000000000000001</v>
@@ -2080,7 +2172,7 @@
         <v>360</v>
       </c>
       <c r="E13" s="0">
-        <v>0.032291899999999998</v>
+        <v>0.031447599999999999</v>
       </c>
       <c r="F13" s="0">
         <v>0.01</v>
@@ -2094,25 +2186,25 @@
     </row>
     <row r="18">
       <c r="B18" s="0" t="s">
-        <v>546</v>
+        <v>574</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>547</v>
+        <v>575</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>548</v>
+        <v>576</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>549</v>
+        <v>577</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>550</v>
+        <v>578</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>551</v>
+        <v>579</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>552</v>
+        <v>580</v>
       </c>
     </row>
     <row r="19">
@@ -2126,7 +2218,7 @@
         <v>1001</v>
       </c>
       <c r="E19" s="0">
-        <v>0.010804100000000001</v>
+        <v>0.0103039</v>
       </c>
       <c r="F19" s="0">
         <v>0.0025000000000000001</v>
@@ -2149,7 +2241,7 @@
         <v>215</v>
       </c>
       <c r="E20" s="0">
-        <v>0.011806499999999999</v>
+        <v>0.011632200000000001</v>
       </c>
       <c r="F20" s="0">
         <v>0.0025000000000000001</v>
@@ -2172,7 +2264,7 @@
         <v>229</v>
       </c>
       <c r="E21" s="0">
-        <v>0.028948700000000001</v>
+        <v>0.025541600000000001</v>
       </c>
       <c r="F21" s="0">
         <v>0.01</v>
@@ -2186,25 +2278,25 @@
     </row>
     <row r="26">
       <c r="B26" s="0" t="s">
-        <v>553</v>
+        <v>581</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>554</v>
+        <v>582</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>555</v>
+        <v>583</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>556</v>
+        <v>584</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>557</v>
+        <v>585</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>558</v>
+        <v>586</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>559</v>
+        <v>587</v>
       </c>
     </row>
     <row r="27">
@@ -2218,7 +2310,7 @@
         <v>270</v>
       </c>
       <c r="E27" s="0">
-        <v>0.0086695000000000001</v>
+        <v>0.0083443000000000007</v>
       </c>
       <c r="F27" s="0">
         <v>0.0025000000000000001</v>
@@ -2241,7 +2333,7 @@
         <v>268</v>
       </c>
       <c r="E28" s="0">
-        <v>0.0110168</v>
+        <v>0.010261599999999999</v>
       </c>
       <c r="F28" s="0">
         <v>0.0025000000000000001</v>
@@ -2264,7 +2356,7 @@
         <v>267</v>
       </c>
       <c r="E29" s="0">
-        <v>0.0263761</v>
+        <v>0.026808499999999999</v>
       </c>
       <c r="F29" s="0">
         <v>0.01</v>

</xml_diff>

<commit_message>
changed critic network and only 8 actions
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -13,7 +13,91 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="616">
+  <si>
+    <t>methodN</t>
+  </si>
+  <si>
+    <t>pathDist</t>
+  </si>
+  <si>
+    <t>numIterations</t>
+  </si>
+  <si>
+    <t>calcTime</t>
+  </si>
+  <si>
+    <t>kGoal</t>
+  </si>
+  <si>
+    <t>kObst</t>
+  </si>
+  <si>
+    <t>rObst</t>
+  </si>
+  <si>
+    <t>methodN</t>
+  </si>
+  <si>
+    <t>pathDist</t>
+  </si>
+  <si>
+    <t>numIterations</t>
+  </si>
+  <si>
+    <t>calcTime</t>
+  </si>
+  <si>
+    <t>kGoal</t>
+  </si>
+  <si>
+    <t>kObst</t>
+  </si>
+  <si>
+    <t>rObst</t>
+  </si>
+  <si>
+    <t>methodN</t>
+  </si>
+  <si>
+    <t>pathDist</t>
+  </si>
+  <si>
+    <t>numIterations</t>
+  </si>
+  <si>
+    <t>calcTime</t>
+  </si>
+  <si>
+    <t>kGoal</t>
+  </si>
+  <si>
+    <t>kObst</t>
+  </si>
+  <si>
+    <t>rObst</t>
+  </si>
+  <si>
+    <t>methodN</t>
+  </si>
+  <si>
+    <t>pathDist</t>
+  </si>
+  <si>
+    <t>numIterations</t>
+  </si>
+  <si>
+    <t>calcTime</t>
+  </si>
+  <si>
+    <t>kGoal</t>
+  </si>
+  <si>
+    <t>kObst</t>
+  </si>
+  <si>
+    <t>rObst</t>
+  </si>
   <si>
     <t>methodN</t>
   </si>
@@ -1797,7 +1881,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="85">
+  <borders count="89">
     <border>
       <left/>
       <right/>
@@ -1889,11 +1973,15 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1979,6 +2067,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="82" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="83" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="84" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="85" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="86" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="87" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="88" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2002,25 +2094,25 @@
   <sheetData>
     <row r="2">
       <c r="B2" s="0" t="s">
-        <v>560</v>
+        <v>588</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>561</v>
+        <v>589</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>562</v>
+        <v>590</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>563</v>
+        <v>591</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>564</v>
+        <v>592</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>565</v>
+        <v>593</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>566</v>
+        <v>594</v>
       </c>
     </row>
     <row r="3">
@@ -2034,7 +2126,7 @@
         <v>281</v>
       </c>
       <c r="E3" s="0">
-        <v>0.1643925</v>
+        <v>0.1479491</v>
       </c>
       <c r="F3" s="0">
         <v>0.0025000000000000001</v>
@@ -2057,7 +2149,7 @@
         <v>306</v>
       </c>
       <c r="E4" s="0">
-        <v>0.015528999999999999</v>
+        <v>0.016117200000000002</v>
       </c>
       <c r="F4" s="0">
         <v>0.0025000000000000001</v>
@@ -2080,7 +2172,7 @@
         <v>355</v>
       </c>
       <c r="E5" s="0">
-        <v>0.023719299999999999</v>
+        <v>0.023758000000000001</v>
       </c>
       <c r="F5" s="0">
         <v>0.01</v>
@@ -2094,25 +2186,25 @@
     </row>
     <row r="10">
       <c r="B10" s="0" t="s">
-        <v>567</v>
+        <v>595</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>568</v>
+        <v>596</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>569</v>
+        <v>597</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>570</v>
+        <v>598</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>571</v>
+        <v>599</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>572</v>
+        <v>600</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>573</v>
+        <v>601</v>
       </c>
     </row>
     <row r="11">
@@ -2126,7 +2218,7 @@
         <v>291</v>
       </c>
       <c r="E11" s="0">
-        <v>0.012711099999999999</v>
+        <v>0.011481399999999999</v>
       </c>
       <c r="F11" s="0">
         <v>0.0025000000000000001</v>
@@ -2149,7 +2241,7 @@
         <v>313</v>
       </c>
       <c r="E12" s="0">
-        <v>0.0225343</v>
+        <v>0.023232800000000001</v>
       </c>
       <c r="F12" s="0">
         <v>0.0025000000000000001</v>
@@ -2172,7 +2264,7 @@
         <v>360</v>
       </c>
       <c r="E13" s="0">
-        <v>0.031447599999999999</v>
+        <v>0.029960299999999999</v>
       </c>
       <c r="F13" s="0">
         <v>0.01</v>
@@ -2186,25 +2278,25 @@
     </row>
     <row r="18">
       <c r="B18" s="0" t="s">
-        <v>574</v>
+        <v>602</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>575</v>
+        <v>603</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>576</v>
+        <v>604</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>577</v>
+        <v>605</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>578</v>
+        <v>606</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>579</v>
+        <v>607</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>580</v>
+        <v>608</v>
       </c>
     </row>
     <row r="19">
@@ -2218,7 +2310,7 @@
         <v>1001</v>
       </c>
       <c r="E19" s="0">
-        <v>0.0103039</v>
+        <v>0.011464</v>
       </c>
       <c r="F19" s="0">
         <v>0.0025000000000000001</v>
@@ -2241,7 +2333,7 @@
         <v>215</v>
       </c>
       <c r="E20" s="0">
-        <v>0.011632200000000001</v>
+        <v>0.0118885</v>
       </c>
       <c r="F20" s="0">
         <v>0.0025000000000000001</v>
@@ -2264,7 +2356,7 @@
         <v>229</v>
       </c>
       <c r="E21" s="0">
-        <v>0.025541600000000001</v>
+        <v>0.024887300000000001</v>
       </c>
       <c r="F21" s="0">
         <v>0.01</v>
@@ -2278,25 +2370,25 @@
     </row>
     <row r="26">
       <c r="B26" s="0" t="s">
-        <v>581</v>
+        <v>609</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>582</v>
+        <v>610</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>583</v>
+        <v>611</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>584</v>
+        <v>612</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>585</v>
+        <v>613</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>586</v>
+        <v>614</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>587</v>
+        <v>615</v>
       </c>
     </row>
     <row r="27">
@@ -2310,7 +2402,7 @@
         <v>270</v>
       </c>
       <c r="E27" s="0">
-        <v>0.0083443000000000007</v>
+        <v>0.0099711000000000001</v>
       </c>
       <c r="F27" s="0">
         <v>0.0025000000000000001</v>
@@ -2333,7 +2425,7 @@
         <v>268</v>
       </c>
       <c r="E28" s="0">
-        <v>0.010261599999999999</v>
+        <v>0.0109009</v>
       </c>
       <c r="F28" s="0">
         <v>0.0025000000000000001</v>
@@ -2356,7 +2448,7 @@
         <v>267</v>
       </c>
       <c r="E29" s="0">
-        <v>0.026808499999999999</v>
+        <v>0.021766000000000001</v>
       </c>
       <c r="F29" s="0">
         <v>0.01</v>

</xml_diff>

<commit_message>
End of EE462 Final Push
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -13,7 +13,91 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="644">
+  <si>
+    <t>methodN</t>
+  </si>
+  <si>
+    <t>pathDist</t>
+  </si>
+  <si>
+    <t>numIterations</t>
+  </si>
+  <si>
+    <t>calcTime</t>
+  </si>
+  <si>
+    <t>kGoal</t>
+  </si>
+  <si>
+    <t>kObst</t>
+  </si>
+  <si>
+    <t>rObst</t>
+  </si>
+  <si>
+    <t>methodN</t>
+  </si>
+  <si>
+    <t>pathDist</t>
+  </si>
+  <si>
+    <t>numIterations</t>
+  </si>
+  <si>
+    <t>calcTime</t>
+  </si>
+  <si>
+    <t>kGoal</t>
+  </si>
+  <si>
+    <t>kObst</t>
+  </si>
+  <si>
+    <t>rObst</t>
+  </si>
+  <si>
+    <t>methodN</t>
+  </si>
+  <si>
+    <t>pathDist</t>
+  </si>
+  <si>
+    <t>numIterations</t>
+  </si>
+  <si>
+    <t>calcTime</t>
+  </si>
+  <si>
+    <t>kGoal</t>
+  </si>
+  <si>
+    <t>kObst</t>
+  </si>
+  <si>
+    <t>rObst</t>
+  </si>
+  <si>
+    <t>methodN</t>
+  </si>
+  <si>
+    <t>pathDist</t>
+  </si>
+  <si>
+    <t>numIterations</t>
+  </si>
+  <si>
+    <t>calcTime</t>
+  </si>
+  <si>
+    <t>kGoal</t>
+  </si>
+  <si>
+    <t>kObst</t>
+  </si>
+  <si>
+    <t>rObst</t>
+  </si>
   <si>
     <t>methodN</t>
   </si>
@@ -1881,7 +1965,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="89">
+  <borders count="93">
     <border>
       <left/>
       <right/>
@@ -1977,11 +2061,15 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -2071,6 +2159,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="86" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="87" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="88" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="89" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="90" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="91" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="92" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2094,25 +2186,25 @@
   <sheetData>
     <row r="2">
       <c r="B2" s="0" t="s">
-        <v>588</v>
+        <v>616</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>589</v>
+        <v>617</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>590</v>
+        <v>618</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>591</v>
+        <v>619</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>592</v>
+        <v>620</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>593</v>
+        <v>621</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>594</v>
+        <v>622</v>
       </c>
     </row>
     <row r="3">
@@ -2126,7 +2218,7 @@
         <v>281</v>
       </c>
       <c r="E3" s="0">
-        <v>0.1479491</v>
+        <v>0.14334710000000001</v>
       </c>
       <c r="F3" s="0">
         <v>0.0025000000000000001</v>
@@ -2149,7 +2241,7 @@
         <v>306</v>
       </c>
       <c r="E4" s="0">
-        <v>0.016117200000000002</v>
+        <v>0.0174301</v>
       </c>
       <c r="F4" s="0">
         <v>0.0025000000000000001</v>
@@ -2172,7 +2264,7 @@
         <v>355</v>
       </c>
       <c r="E5" s="0">
-        <v>0.023758000000000001</v>
+        <v>0.031169100000000002</v>
       </c>
       <c r="F5" s="0">
         <v>0.01</v>
@@ -2186,25 +2278,25 @@
     </row>
     <row r="10">
       <c r="B10" s="0" t="s">
-        <v>595</v>
+        <v>623</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>596</v>
+        <v>624</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>597</v>
+        <v>625</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>598</v>
+        <v>626</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>599</v>
+        <v>627</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>600</v>
+        <v>628</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>601</v>
+        <v>629</v>
       </c>
     </row>
     <row r="11">
@@ -2218,7 +2310,7 @@
         <v>291</v>
       </c>
       <c r="E11" s="0">
-        <v>0.011481399999999999</v>
+        <v>0.013315799999999999</v>
       </c>
       <c r="F11" s="0">
         <v>0.0025000000000000001</v>
@@ -2241,7 +2333,7 @@
         <v>313</v>
       </c>
       <c r="E12" s="0">
-        <v>0.023232800000000001</v>
+        <v>0.0260559</v>
       </c>
       <c r="F12" s="0">
         <v>0.0025000000000000001</v>
@@ -2264,7 +2356,7 @@
         <v>360</v>
       </c>
       <c r="E13" s="0">
-        <v>0.029960299999999999</v>
+        <v>0.031995999999999997</v>
       </c>
       <c r="F13" s="0">
         <v>0.01</v>
@@ -2278,25 +2370,25 @@
     </row>
     <row r="18">
       <c r="B18" s="0" t="s">
-        <v>602</v>
+        <v>630</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>603</v>
+        <v>631</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>604</v>
+        <v>632</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>605</v>
+        <v>633</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>606</v>
+        <v>634</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>607</v>
+        <v>635</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>608</v>
+        <v>636</v>
       </c>
     </row>
     <row r="19">
@@ -2310,7 +2402,7 @@
         <v>1001</v>
       </c>
       <c r="E19" s="0">
-        <v>0.011464</v>
+        <v>0.012299600000000001</v>
       </c>
       <c r="F19" s="0">
         <v>0.0025000000000000001</v>
@@ -2333,7 +2425,7 @@
         <v>215</v>
       </c>
       <c r="E20" s="0">
-        <v>0.0118885</v>
+        <v>0.0134176</v>
       </c>
       <c r="F20" s="0">
         <v>0.0025000000000000001</v>
@@ -2356,7 +2448,7 @@
         <v>229</v>
       </c>
       <c r="E21" s="0">
-        <v>0.024887300000000001</v>
+        <v>0.027660899999999999</v>
       </c>
       <c r="F21" s="0">
         <v>0.01</v>
@@ -2370,25 +2462,25 @@
     </row>
     <row r="26">
       <c r="B26" s="0" t="s">
-        <v>609</v>
+        <v>637</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>610</v>
+        <v>638</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>611</v>
+        <v>639</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>612</v>
+        <v>640</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>613</v>
+        <v>641</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>614</v>
+        <v>642</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>615</v>
+        <v>643</v>
       </c>
     </row>
     <row r="27">
@@ -2402,7 +2494,7 @@
         <v>270</v>
       </c>
       <c r="E27" s="0">
-        <v>0.0099711000000000001</v>
+        <v>0.0090486000000000004</v>
       </c>
       <c r="F27" s="0">
         <v>0.0025000000000000001</v>
@@ -2425,7 +2517,7 @@
         <v>268</v>
       </c>
       <c r="E28" s="0">
-        <v>0.0109009</v>
+        <v>0.0122129</v>
       </c>
       <c r="F28" s="0">
         <v>0.0025000000000000001</v>
@@ -2448,7 +2540,7 @@
         <v>267</v>
       </c>
       <c r="E29" s="0">
-        <v>0.021766000000000001</v>
+        <v>0.028326</v>
       </c>
       <c r="F29" s="0">
         <v>0.01</v>

</xml_diff>